<commit_message>
ES6 적용, connection pool 적용
</commit_message>
<xml_diff>
--- a/dist/uploads/excel/fail_upload.xlsx
+++ b/dist/uploads/excel/fail_upload.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>지점명</t>
   </si>
@@ -31,274 +31,34 @@
     <t>미입력사유</t>
   </si>
   <si>
-    <t>서귀포점</t>
+    <t>양재점</t>
+  </si>
+  <si>
+    <t>점주</t>
+  </si>
+  <si>
+    <t>점주(양재)</t>
+  </si>
+  <si>
+    <t>01099999999</t>
+  </si>
+  <si>
+    <t>yangje@example.com</t>
+  </si>
+  <si>
+    <t>휴대폰번호 중복,이메일 중복</t>
+  </si>
+  <si>
+    <t>사원</t>
+  </si>
+  <si>
+    <t>사원(양재)</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>박광균</t>
-  </si>
-  <si>
-    <t>01086627071</t>
-  </si>
-  <si>
-    <t>doublek17@hanmail.net</t>
-  </si>
-  <si>
-    <t>필수입력값 누락,휴대폰번호 중복,이메일 중복</t>
-  </si>
-  <si>
-    <t>남악점</t>
-  </si>
-  <si>
-    <t>점주</t>
-  </si>
-  <si>
-    <t>정병훈</t>
-  </si>
-  <si>
-    <t>01041021879</t>
-  </si>
-  <si>
-    <t>voda77@naver.com</t>
-  </si>
-  <si>
-    <t>휴대폰번호 중복,이메일 중복</t>
-  </si>
-  <si>
-    <t>미장점</t>
-  </si>
-  <si>
-    <t>서명주</t>
-  </si>
-  <si>
-    <t>010431140821</t>
-  </si>
-  <si>
-    <t>poohru@hanmail.net</t>
-  </si>
-  <si>
-    <t>잘못된 휴대폰번호 형식,이메일 중복</t>
-  </si>
-  <si>
-    <t>방이점</t>
-  </si>
-  <si>
-    <t>김은경</t>
-  </si>
-  <si>
-    <t>01056578077</t>
-  </si>
-  <si>
-    <t>tov10</t>
-  </si>
-  <si>
-    <t>잘못된 이메일 형식,휴대폰번호 중복</t>
-  </si>
-  <si>
-    <t>군포점</t>
-  </si>
-  <si>
-    <t>김남율</t>
-  </si>
-  <si>
-    <t>01041714222</t>
-  </si>
-  <si>
-    <t>kny1003y@naver.com</t>
-  </si>
-  <si>
-    <t>상암점</t>
-  </si>
-  <si>
-    <t>정춘영</t>
-  </si>
-  <si>
-    <t>01094917643</t>
-  </si>
-  <si>
-    <t>chunpung1@naver.com</t>
-  </si>
-  <si>
-    <t>전주점</t>
-  </si>
-  <si>
-    <t>오현진</t>
-  </si>
-  <si>
-    <t>01024473443</t>
-  </si>
-  <si>
-    <t>eyeohj@naver.com</t>
-  </si>
-  <si>
-    <t>강릉점</t>
-  </si>
-  <si>
-    <t>이인영</t>
-  </si>
-  <si>
-    <t>01044541471</t>
-  </si>
-  <si>
-    <t>voda2580@naver.com</t>
-  </si>
-  <si>
-    <t>신흥점</t>
-  </si>
-  <si>
-    <t>문응기</t>
-  </si>
-  <si>
-    <t>01032608283</t>
-  </si>
-  <si>
-    <t>m2k0913@hanmail.net</t>
-  </si>
-  <si>
-    <t>정읍점</t>
-  </si>
-  <si>
-    <t>박순희</t>
-  </si>
-  <si>
-    <t>01036568185</t>
-  </si>
-  <si>
-    <t>enffl1173@naver.com</t>
-  </si>
-  <si>
-    <t>구의점</t>
-  </si>
-  <si>
-    <t>김정표</t>
-  </si>
-  <si>
-    <t>01087848071</t>
-  </si>
-  <si>
-    <t>e709_@hanmail.net</t>
-  </si>
-  <si>
-    <t>목동점</t>
-  </si>
-  <si>
-    <t>이희환</t>
-  </si>
-  <si>
-    <t>01034032969</t>
-  </si>
-  <si>
-    <t>hwan75the@naver.com</t>
-  </si>
-  <si>
-    <t>분당정자점</t>
-  </si>
-  <si>
-    <t>박성열</t>
-  </si>
-  <si>
-    <t>01090758090</t>
-  </si>
-  <si>
-    <t>jungja_voda@naver.com</t>
-  </si>
-  <si>
-    <t>광교점</t>
-  </si>
-  <si>
-    <t>최우영</t>
-  </si>
-  <si>
-    <t>01087890196</t>
-  </si>
-  <si>
-    <t>voda0401@naver.com</t>
-  </si>
-  <si>
-    <t>야탑점</t>
-  </si>
-  <si>
-    <t>김지연</t>
-  </si>
-  <si>
-    <t>01063991741</t>
-  </si>
-  <si>
-    <t>abba2111@naver.com</t>
-  </si>
-  <si>
-    <t>군산점</t>
-  </si>
-  <si>
-    <t>최순웅</t>
-  </si>
-  <si>
-    <t>01020091407</t>
-  </si>
-  <si>
-    <t>voda113@hanmail.net</t>
-  </si>
-  <si>
-    <t>세종첫마을점</t>
-  </si>
-  <si>
-    <t>서봉근</t>
-  </si>
-  <si>
-    <t>01089995865</t>
-  </si>
-  <si>
-    <t>hwarang1972@naver.com</t>
-  </si>
-  <si>
-    <t>수지점</t>
-  </si>
-  <si>
-    <t>김성우</t>
-  </si>
-  <si>
-    <t>01082912468</t>
-  </si>
-  <si>
-    <t>sung-woo7655@hanmail.net</t>
-  </si>
-  <si>
-    <t>송파점</t>
-  </si>
-  <si>
-    <t>구창모</t>
-  </si>
-  <si>
-    <t>01097620828</t>
-  </si>
-  <si>
-    <t>lucas@intertoday.com</t>
-  </si>
-  <si>
-    <t>일원본점</t>
-  </si>
-  <si>
-    <t>배진호</t>
-  </si>
-  <si>
-    <t>01085662702</t>
-  </si>
-  <si>
-    <t>bjh9407@hanmail.net</t>
-  </si>
-  <si>
-    <t>세종아름점</t>
-  </si>
-  <si>
-    <t>김용준</t>
-  </si>
-  <si>
-    <t>01030111103</t>
-  </si>
-  <si>
-    <t>kyj-0921@daum.net</t>
+    <t>필수입력값 누락,잘못된 이메일 형식,잘못된 휴대폰번호 형식</t>
   </si>
 </sst>
 </file>
@@ -737,404 +497,43 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" t="s">
-        <v>17</v>
-      </c>
-    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25"/>

</xml_diff>